<commit_message>
adding changes to the file
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2129135\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025D5FD2-6DEB-4CFF-93AE-EFCA6D8E95DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396F6718-76B7-4B94-8AF9-C99370835253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{51674F4F-AF69-479A-8C93-B203ECD79E6E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>manual steps</t>
   </si>
@@ -96,13 +96,36 @@
   </si>
   <si>
     <t>Update relevant documentation to reflect the changes made in the target org, including new custom objects, fields, and processes. </t>
+  </si>
+  <si>
+    <r>
+      <t>Merging Branches in a Local RepositoryTo merge branches locally, use </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF040C28"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>git checkout to switch to the branch you want to merge into</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. This branch is typically the main branch. Next, use git merge and specify the name of the other branch to bring into this branch.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +143,18 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF001D35"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF040C28"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -144,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -155,6 +190,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86DBC1B2-0BC6-432A-BFD1-6DCD26CC4D6E}">
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -500,74 +536,77 @@
     <col min="1" max="1" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:1" ht="42" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="28" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:1" ht="42" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="28" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="28" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:1" ht="28" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="28" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="28" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="28" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:1" ht="28" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="28" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>

</xml_diff>